<commit_message>
report/list implemented and JSON answer of turn/list switched to Array
</commit_message>
<xml_diff>
--- a/docs/routes.xlsx
+++ b/docs/routes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>Route</t>
   </si>
@@ -168,6 +168,27 @@
   </si>
   <si>
     <t>{"success":true,"report":###,"message":"Report aperto con successo"}</t>
+  </si>
+  <si>
+    <t>/report/list</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>ora_apertura</t>
+  </si>
+  <si>
+    <t>ora_chiusura</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>[{"id":8,"data":"30/03/16","ora_apertura":"00:43:30","ora_chiusura":null,"note":null}, … ]</t>
+  </si>
+  <si>
+    <t>{"code":401,"error":"Not authorized to retrieve specified turn"}</t>
   </si>
 </sst>
 </file>
@@ -425,15 +446,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -444,117 +459,141 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -836,426 +875,588 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:K25"/>
+  <dimension ref="C5:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="3.73046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.73046875" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.06640625" style="2"/>
+    <col min="5" max="5" width="9.06640625" style="1"/>
     <col min="6" max="6" width="12.06640625" customWidth="1"/>
-    <col min="7" max="8" width="9.06640625" style="2"/>
-    <col min="9" max="9" width="11.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="22.1328125" customWidth="1"/>
-    <col min="11" max="11" width="70.73046875" customWidth="1"/>
+    <col min="7" max="8" width="9.06640625" style="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.06640625" customWidth="1"/>
+    <col min="11" max="11" width="73.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C6" s="29">
+      <c r="C6" s="11">
         <v>1</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="30">
         <v>200</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="32" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C7" s="30">
+      <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="36" t="s">
+      <c r="D7" s="36"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4" t="s">
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="11"/>
+      <c r="K7" s="46"/>
     </row>
     <row r="8" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C8" s="30">
+      <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="36" t="s">
+      <c r="D8" s="36"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="4" t="s">
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="K8" s="46"/>
     </row>
     <row r="9" spans="3:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C9" s="30">
+      <c r="C9" s="12">
         <v>1</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="36" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="30">
         <v>400</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C10" s="30">
+      <c r="C10" s="12">
         <v>1</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="36" t="s">
+      <c r="D10" s="36"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="4" t="s">
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="16"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C11" s="31">
+      <c r="C11" s="13">
         <v>1</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="4" t="s">
+      <c r="D11" s="37"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="16"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C12" s="29">
+      <c r="C12" s="11">
         <v>2</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="30">
         <v>200</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K12" s="32" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C13" s="30">
+      <c r="C13" s="12">
         <v>2</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="6" t="s">
+      <c r="D13" s="36"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K13" s="11"/>
+      <c r="K13" s="46"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C14" s="30">
+      <c r="C14" s="12">
         <v>2</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="6" t="s">
+      <c r="D14" s="36"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K14" s="11"/>
+      <c r="K14" s="46"/>
     </row>
     <row r="15" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C15" s="31">
+      <c r="C15" s="13">
         <v>2</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="6" t="s">
+      <c r="D15" s="37"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="11"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C16" s="29">
+      <c r="C16" s="11">
         <v>3</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="30">
         <v>200</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="24" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C17" s="30">
+      <c r="C17" s="12">
         <v>3</v>
       </c>
       <c r="D17" s="39"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="6" t="s">
+      <c r="E17" s="42"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="16"/>
+      <c r="K17" s="25"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C18" s="30">
+      <c r="C18" s="12">
         <v>3</v>
       </c>
       <c r="D18" s="39"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="6" t="s">
+      <c r="E18" s="42"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K18" s="16"/>
+      <c r="K18" s="25"/>
     </row>
     <row r="19" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C19" s="31">
+      <c r="C19" s="13">
         <v>3</v>
       </c>
       <c r="D19" s="40"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="21" t="s">
+      <c r="E19" s="43"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="17"/>
+      <c r="K19" s="26"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C20" s="29">
+      <c r="C20" s="11">
         <v>4</v>
       </c>
       <c r="D20" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="30">
         <v>200</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="44" t="s">
+      <c r="J20" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C21" s="30">
+      <c r="C21" s="12">
         <v>4</v>
       </c>
       <c r="D21" s="39"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="47" t="s">
+      <c r="E21" s="28"/>
+      <c r="F21" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="28" t="s">
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K21" s="16"/>
+      <c r="K21" s="25"/>
     </row>
     <row r="22" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C22" s="30">
+      <c r="C22" s="12">
         <v>4</v>
       </c>
       <c r="D22" s="39"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="45" t="s">
+      <c r="E22" s="28"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="K22" s="17"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="C23" s="30">
+      <c r="C23" s="12">
         <v>4</v>
       </c>
       <c r="D23" s="39"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="8" t="s">
+      <c r="E23" s="28"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="30">
         <v>401</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="9" t="s">
+      <c r="J23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="K23" s="32" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C24" s="31">
+      <c r="C24" s="13">
         <v>4</v>
       </c>
       <c r="D24" s="40"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="13" t="s">
+      <c r="E24" s="29"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="14"/>
+      <c r="K24" s="33"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.45">
-      <c r="E25" s="1"/>
+      <c r="C25" s="14">
+        <v>5</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="30">
+        <v>200</v>
+      </c>
+      <c r="I25" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C26" s="15">
+        <v>5</v>
+      </c>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="28"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="25"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C27" s="15">
+        <v>5</v>
+      </c>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="K27" s="25"/>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C28" s="15">
+        <v>5</v>
+      </c>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" s="25"/>
+    </row>
+    <row r="29" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C29" s="15">
+        <v>5</v>
+      </c>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="K29" s="26"/>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="C30" s="15">
+        <v>5</v>
+      </c>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="30">
+        <v>401</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C31" s="16">
+        <v>5</v>
+      </c>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="26"/>
     </row>
   </sheetData>
   <autoFilter ref="D5:K22"/>
-  <mergeCells count="34">
+  <mergeCells count="44">
+    <mergeCell ref="E25:E31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="K25:K29"/>
+    <mergeCell ref="I25:I29"/>
+    <mergeCell ref="H25:H29"/>
+    <mergeCell ref="G25:G29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="G12:G15"/>
     <mergeCell ref="K20:K22"/>
     <mergeCell ref="E20:E24"/>
     <mergeCell ref="G23:G24"/>
@@ -1264,32 +1465,6 @@
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="I20:I22"/>
     <mergeCell ref="H20:H22"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="E6:E11"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>